<commit_message>
Saving results and OLS
</commit_message>
<xml_diff>
--- a/NIFTY50 simulations/results_cost.xlsx
+++ b/NIFTY50 simulations/results_cost.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarthakbajaj/Indicators/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarthakbajaj/Indicators/NIFTY50 simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28609,7 +28609,7 @@
         <v>66</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:I45" si="0">IF(C3&gt;0,1,0)</f>
+        <f t="shared" ref="G3:G45" si="0">IF(C3&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="H3" t="str">
@@ -29975,7 +29975,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I49"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30015,7 +30015,7 @@
         <v>159</v>
       </c>
       <c r="K1">
-        <f>IF(C1&gt;0,1,0)</f>
+        <f t="shared" ref="K1:K32" si="0">IF(C1&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -30027,7 +30027,7 @@
         <v>157</v>
       </c>
       <c r="C2">
-        <v>0.32928629486</v>
+        <v>0.29728629486000002</v>
       </c>
       <c r="D2">
         <v>0.214429804306</v>
@@ -30039,7 +30039,7 @@
         <v>69</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G49" si="0">LEFT(A2,LEN(A2)-2)</f>
+        <f t="shared" ref="G2:G49" si="1">LEFT(A2,LEN(A2)-2)</f>
         <v>ADANIPORTS</v>
       </c>
       <c r="H2">
@@ -30047,14 +30047,14 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I49" si="1">IF(H2=1,C2,"")</f>
-        <v>0.32928629486</v>
+        <f t="shared" ref="I2:I49" si="2">IF(H2=1,C2,"")</f>
+        <v>0.29728629486000002</v>
       </c>
       <c r="J2" t="s">
         <v>160</v>
       </c>
       <c r="K2">
-        <f>IF(C2&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30078,7 +30078,7 @@
         <v>70</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>AMBUJACEM</v>
       </c>
       <c r="H3">
@@ -30086,14 +30086,14 @@
         <v>0</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J3" t="s">
         <v>161</v>
       </c>
       <c r="K3">
-        <f>IF(C3&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30117,7 +30117,7 @@
         <v>60</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ASIANPAINT</v>
       </c>
       <c r="H4">
@@ -30125,14 +30125,14 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.13379479313000001</v>
       </c>
       <c r="J4" t="s">
         <v>162</v>
       </c>
       <c r="K4">
-        <f>IF(C4&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30156,7 +30156,7 @@
         <v>75</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>AUROPHARMA</v>
       </c>
       <c r="H5">
@@ -30164,14 +30164,14 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21134557251</v>
       </c>
       <c r="J5" t="s">
         <v>163</v>
       </c>
       <c r="K5">
-        <f>IF(C5&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30195,7 +30195,7 @@
         <v>77</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>AXISBANK</v>
       </c>
       <c r="H6">
@@ -30203,14 +30203,14 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43202267813599998</v>
       </c>
       <c r="J6" t="s">
         <v>164</v>
       </c>
       <c r="K6">
-        <f>IF(C6&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30234,7 +30234,7 @@
         <v>67</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>BAJAJ-AUTO</v>
       </c>
       <c r="H7">
@@ -30242,14 +30242,14 @@
         <v>0</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J7" t="s">
         <v>165</v>
       </c>
       <c r="K7">
-        <f>IF(C7&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30273,7 +30273,7 @@
         <v>64</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>BANKBARODA</v>
       </c>
       <c r="H8">
@@ -30281,14 +30281,14 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.123897374367</v>
       </c>
       <c r="J8" t="s">
         <v>166</v>
       </c>
       <c r="K8">
-        <f>IF(C8&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30312,7 +30312,7 @@
         <v>64</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>BHARTIARTL</v>
       </c>
       <c r="H9">
@@ -30320,14 +30320,14 @@
         <v>0</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J9" t="s">
         <v>167</v>
       </c>
       <c r="K9">
-        <f>IF(C9&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30351,7 +30351,7 @@
         <v>79</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>BOSCHLTD</v>
       </c>
       <c r="H10">
@@ -30359,14 +30359,14 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.71965432705099996</v>
       </c>
       <c r="J10" t="s">
         <v>168</v>
       </c>
       <c r="K10">
-        <f>IF(C10&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30390,7 +30390,7 @@
         <v>75</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>BPCL</v>
       </c>
       <c r="H11">
@@ -30398,14 +30398,14 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22030132742200001</v>
       </c>
       <c r="J11" t="s">
         <v>169</v>
       </c>
       <c r="K11">
-        <f>IF(C11&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30429,7 +30429,7 @@
         <v>69</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CIPLA</v>
       </c>
       <c r="H12">
@@ -30437,14 +30437,14 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14527870335400001</v>
       </c>
       <c r="J12" t="s">
         <v>170</v>
       </c>
       <c r="K12">
-        <f>IF(C12&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30468,7 +30468,7 @@
         <v>66</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>COALINDIA</v>
       </c>
       <c r="H13">
@@ -30476,14 +30476,14 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18601663246899999</v>
       </c>
       <c r="J13" t="s">
         <v>171</v>
       </c>
       <c r="K13">
-        <f>IF(C13&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30507,7 +30507,7 @@
         <v>72</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DRREDDY</v>
       </c>
       <c r="H14">
@@ -30515,14 +30515,14 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83477371906300002</v>
       </c>
       <c r="J14" t="s">
         <v>172</v>
       </c>
       <c r="K14">
-        <f>IF(C14&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30546,7 +30546,7 @@
         <v>72</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>EICHERMOT</v>
       </c>
       <c r="H15">
@@ -30554,14 +30554,14 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70181999939999995</v>
       </c>
       <c r="J15" t="s">
         <v>173</v>
       </c>
       <c r="K15">
-        <f>IF(C15&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30585,7 +30585,7 @@
         <v>70</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>GAIL</v>
       </c>
       <c r="H16">
@@ -30593,14 +30593,14 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47392177569499999</v>
       </c>
       <c r="J16" t="s">
         <v>174</v>
       </c>
       <c r="K16">
-        <f>IF(C16&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30624,7 +30624,7 @@
         <v>69</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HCLTECH</v>
       </c>
       <c r="H17">
@@ -30632,14 +30632,14 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.9487102854600002E-2</v>
       </c>
       <c r="J17" t="s">
         <v>175</v>
       </c>
       <c r="K17">
-        <f>IF(C17&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30663,7 +30663,7 @@
         <v>70</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HDFC</v>
       </c>
       <c r="H18">
@@ -30671,14 +30671,14 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.5759582731599999E-2</v>
       </c>
       <c r="J18" t="s">
         <v>176</v>
       </c>
       <c r="K18">
-        <f>IF(C18&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30702,7 +30702,7 @@
         <v>59</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HDFCBANK</v>
       </c>
       <c r="H19">
@@ -30710,14 +30710,14 @@
         <v>0</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J19" t="s">
         <v>177</v>
       </c>
       <c r="K19">
-        <f>IF(C19&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30741,7 +30741,7 @@
         <v>65</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HEROMOTOCO</v>
       </c>
       <c r="H20">
@@ -30749,14 +30749,14 @@
         <v>0</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J20" t="s">
         <v>178</v>
       </c>
       <c r="K20">
-        <f>IF(C20&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30780,7 +30780,7 @@
         <v>68</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HINDALCO</v>
       </c>
       <c r="H21">
@@ -30788,14 +30788,14 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.28189185926900001</v>
       </c>
       <c r="J21" t="s">
         <v>179</v>
       </c>
       <c r="K21">
-        <f>IF(C21&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30819,7 +30819,7 @@
         <v>66</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HINDUNILVR</v>
       </c>
       <c r="H22">
@@ -30827,14 +30827,14 @@
         <v>0</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J22" t="s">
         <v>180</v>
       </c>
       <c r="K22">
-        <f>IF(C22&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30858,7 +30858,7 @@
         <v>67</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>IBULHSGFIN</v>
       </c>
       <c r="H23">
@@ -30866,14 +30866,14 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.40752798777400001</v>
       </c>
       <c r="J23" t="s">
         <v>181</v>
       </c>
       <c r="K23">
-        <f>IF(C23&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30897,7 +30897,7 @@
         <v>74</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ICICIBANK</v>
       </c>
       <c r="H24">
@@ -30905,14 +30905,14 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.226891781712</v>
       </c>
       <c r="J24" t="s">
         <v>182</v>
       </c>
       <c r="K24">
-        <f>IF(C24&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30936,7 +30936,7 @@
         <v>72</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INDUSINDBK</v>
       </c>
       <c r="H25">
@@ -30944,14 +30944,14 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.12027814894E-2</v>
       </c>
       <c r="J25" t="s">
         <v>183</v>
       </c>
       <c r="K25">
-        <f>IF(C25&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30975,7 +30975,7 @@
         <v>65</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INFY</v>
       </c>
       <c r="H26">
@@ -30983,14 +30983,14 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2811103483899998E-2</v>
       </c>
       <c r="J26" t="s">
         <v>184</v>
       </c>
       <c r="K26">
-        <f>IF(C26&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -31014,7 +31014,7 @@
         <v>66</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>IOC</v>
       </c>
       <c r="H27">
@@ -31022,14 +31022,14 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.198696374446</v>
       </c>
       <c r="J27" t="s">
         <v>185</v>
       </c>
       <c r="K27">
-        <f>IF(C27&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31053,7 +31053,7 @@
         <v>66</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ITC</v>
       </c>
       <c r="H28">
@@ -31061,14 +31061,14 @@
         <v>0</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J28" t="s">
         <v>186</v>
       </c>
       <c r="K28">
-        <f>IF(C28&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -31092,7 +31092,7 @@
         <v>58</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>KOTAKBANK</v>
       </c>
       <c r="H29">
@@ -31100,14 +31100,14 @@
         <v>0</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J29" t="s">
         <v>187</v>
       </c>
       <c r="K29">
-        <f>IF(C29&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31131,7 +31131,7 @@
         <v>78</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>LT</v>
       </c>
       <c r="H30">
@@ -31139,14 +31139,14 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24457347954299999</v>
       </c>
       <c r="J30" t="s">
         <v>188</v>
       </c>
       <c r="K30">
-        <f>IF(C30&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -31170,7 +31170,7 @@
         <v>67</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>LUPIN</v>
       </c>
       <c r="H31">
@@ -31178,14 +31178,14 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34770891177899999</v>
       </c>
       <c r="J31" t="s">
         <v>189</v>
       </c>
       <c r="K31">
-        <f>IF(C31&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -31209,7 +31209,7 @@
         <v>67</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M&amp;M</v>
       </c>
       <c r="H32">
@@ -31217,14 +31217,14 @@
         <v>0</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J32" t="s">
         <v>190</v>
       </c>
       <c r="K32">
-        <f>IF(C32&gt;0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -31248,7 +31248,7 @@
         <v>64</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>MARUTI</v>
       </c>
       <c r="H33">
@@ -31256,14 +31256,14 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.302114807313</v>
       </c>
       <c r="J33" t="s">
         <v>191</v>
       </c>
       <c r="K33">
-        <f>IF(C33&gt;0,1,0)</f>
+        <f t="shared" ref="K33:K49" si="3">IF(C33&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -31287,7 +31287,7 @@
         <v>75</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>NTPC</v>
       </c>
       <c r="H34">
@@ -31295,14 +31295,14 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.230393366563</v>
       </c>
       <c r="J34" t="s">
         <v>192</v>
       </c>
       <c r="K34">
-        <f>IF(C34&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31326,7 +31326,7 @@
         <v>64</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ONGC</v>
       </c>
       <c r="H35">
@@ -31334,14 +31334,14 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.51193596412300002</v>
       </c>
       <c r="J35" t="s">
         <v>193</v>
       </c>
       <c r="K35">
-        <f>IF(C35&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31365,7 +31365,7 @@
         <v>64</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>POWERGRID</v>
       </c>
       <c r="H36">
@@ -31373,14 +31373,14 @@
         <v>0</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J36" t="s">
         <v>194</v>
       </c>
       <c r="K36">
-        <f>IF(C36&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31404,7 +31404,7 @@
         <v>73</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>RELIANCE</v>
       </c>
       <c r="H37">
@@ -31412,14 +31412,14 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30171269321100003</v>
       </c>
       <c r="J37" t="s">
         <v>195</v>
       </c>
       <c r="K37">
-        <f>IF(C37&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31443,7 +31443,7 @@
         <v>68</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SBIN</v>
       </c>
       <c r="H38">
@@ -31451,14 +31451,14 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.132783105421</v>
       </c>
       <c r="J38" t="s">
         <v>196</v>
       </c>
       <c r="K38">
-        <f>IF(C38&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31482,7 +31482,7 @@
         <v>71</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SUNPHARMA</v>
       </c>
       <c r="H39">
@@ -31490,14 +31490,14 @@
         <v>0</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J39" t="s">
         <v>197</v>
       </c>
       <c r="K39">
-        <f>IF(C39&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31521,7 +31521,7 @@
         <v>71</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TATAMOTORS</v>
       </c>
       <c r="H40">
@@ -31529,14 +31529,14 @@
         <v>0</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J40" t="s">
         <v>198</v>
       </c>
       <c r="K40">
-        <f>IF(C40&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31560,7 +31560,7 @@
         <v>73</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TATAMTRDVR</v>
       </c>
       <c r="H41">
@@ -31568,14 +31568,14 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.27295800432200001</v>
       </c>
       <c r="J41" t="s">
         <v>199</v>
       </c>
       <c r="K41">
-        <f>IF(C41&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31599,7 +31599,7 @@
         <v>70</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TATAPOWER</v>
       </c>
       <c r="H42">
@@ -31607,14 +31607,14 @@
         <v>1</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.14184802676800001</v>
       </c>
       <c r="J42" t="s">
         <v>200</v>
       </c>
       <c r="K42">
-        <f>IF(C42&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31638,7 +31638,7 @@
         <v>74</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TATASTEEL</v>
       </c>
       <c r="H43">
@@ -31646,14 +31646,14 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.537272225715</v>
       </c>
       <c r="J43" t="s">
         <v>201</v>
       </c>
       <c r="K43">
-        <f>IF(C43&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31677,7 +31677,7 @@
         <v>68</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TCS</v>
       </c>
       <c r="H44">
@@ -31685,14 +31685,14 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.2616778093300003E-2</v>
       </c>
       <c r="J44" t="s">
         <v>202</v>
       </c>
       <c r="K44">
-        <f>IF(C44&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31716,7 +31716,7 @@
         <v>74</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TECHM</v>
       </c>
       <c r="H45">
@@ -31724,14 +31724,14 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37647996778199999</v>
       </c>
       <c r="J45" t="s">
         <v>203</v>
       </c>
       <c r="K45">
-        <f>IF(C45&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31755,7 +31755,7 @@
         <v>73</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ULTRACEMCO</v>
       </c>
       <c r="H46">
@@ -31763,14 +31763,14 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30378051315499999</v>
       </c>
       <c r="J46" t="s">
         <v>204</v>
       </c>
       <c r="K46">
-        <f>IF(C46&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31794,7 +31794,7 @@
         <v>65</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WIPRO</v>
       </c>
       <c r="H47">
@@ -31802,14 +31802,14 @@
         <v>0</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J47" t="s">
         <v>205</v>
       </c>
       <c r="K47">
-        <f>IF(C47&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31833,7 +31833,7 @@
         <v>73</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>YESBANK</v>
       </c>
       <c r="H48">
@@ -31841,14 +31841,14 @@
         <v>1</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25747797257400001</v>
       </c>
       <c r="J48" t="s">
         <v>206</v>
       </c>
       <c r="K48">
-        <f>IF(C48&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31872,7 +31872,7 @@
         <v>65</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ZEEL</v>
       </c>
       <c r="H49">
@@ -31880,14 +31880,14 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18335481280900001</v>
       </c>
       <c r="J49" t="s">
         <v>207</v>
       </c>
       <c r="K49">
-        <f>IF(C49&gt;0,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>